<commit_message>
fix stanza template example
</commit_message>
<xml_diff>
--- a/RCaNmodel/inst/extdata/CaN_template_mini_stanza.xlsx
+++ b/RCaNmodel/inst/extdata/CaN_template_mini_stanza.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
   <si>
     <t xml:space="preserve">Template for input data to CaN models</t>
   </si>
@@ -147,9 +147,6 @@
     <t xml:space="preserve">F08</t>
   </si>
   <si>
-    <t xml:space="preserve">F09</t>
-  </si>
-  <si>
     <t xml:space="preserve">Year</t>
   </si>
   <si>
@@ -232,6 +229,30 @@
   </si>
   <si>
     <t xml:space="preserve">RecruitmentHerbZooplankton0&lt;=20000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HerbZooplankton&lt;=3*HerbZooplankton_Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HerbZooplankton&gt;=0.1*HerbZooplankton_Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OmniZooplankton&lt;=3*OmniZooplankton_Biomass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OmniZooplankton&gt;=0.1*OmniZooplankton_Biomass</t>
   </si>
 </sst>
 </file>
@@ -308,7 +329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -318,10 +339,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -348,7 +365,7 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -449,10 +466,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="141" zoomScaleNormal="141" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="8.36"/>
   </cols>
@@ -585,7 +602,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="1023" style="1" width="8.36"/>
   </cols>
@@ -686,13 +703,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="189" zoomScaleNormal="189" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -748,7 +765,7 @@
       <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="3" t="b">
+      <c r="D4" s="0" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -763,26 +780,12 @@
       <c r="C5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="3" t="b">
+      <c r="D5" s="0" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="3" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -802,10 +805,10 @@
   <dimension ref="A1:M1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="153" zoomScaleNormal="153" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.34"/>
@@ -824,43 +827,43 @@
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,40 +1068,40 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="215" zoomScaleNormal="215" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>1</v>
@@ -1106,13 +1109,13 @@
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -1120,13 +1123,13 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -1134,13 +1137,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>1</v>
@@ -1148,18 +1151,75 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="B7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>